<commit_message>
updated example data, added new example data: get_hr_subject_data_dict_example()
</commit_message>
<xml_diff>
--- a/example_data/ecg_time_log.xlsx
+++ b/example_data/ecg_time_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10606"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richer/Documents/PhD/Projects/BioPsyKit/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F5EAD3-4452-E647-8285-0E687666A545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D8AB64-225C-B24A-990D-512D360181EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,12 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
     <t>End</t>
   </si>
   <si>
@@ -50,6 +44,12 @@
   </si>
   <si>
     <t>Vp02</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>condition</t>
   </si>
 </sst>
 </file>
@@ -331,7 +331,7 @@
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -341,33 +341,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>0.52228009259259256</v>
@@ -387,10 +387,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2">
         <v>0.5380787037037037</v>

</xml_diff>